<commit_message>
Added in trial header names
</commit_message>
<xml_diff>
--- a/RPM_verification/RPM_data.xlsx
+++ b/RPM_verification/RPM_data.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merc.MERCURY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merc.MERCURY\Documents\project-g-force\RPM_verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
     <sheet name="Results T2" sheetId="17" r:id="rId2"/>
     <sheet name="Results T3" sheetId="18" r:id="rId3"/>
-    <sheet name="30" sheetId="1" r:id="rId4"/>
-    <sheet name="50" sheetId="2" r:id="rId5"/>
-    <sheet name="70" sheetId="3" r:id="rId6"/>
-    <sheet name="90" sheetId="4" r:id="rId7"/>
-    <sheet name="150" sheetId="5" r:id="rId8"/>
+    <sheet name="30T1" sheetId="1" r:id="rId4"/>
+    <sheet name="50T1" sheetId="2" r:id="rId5"/>
+    <sheet name="70T1" sheetId="3" r:id="rId6"/>
+    <sheet name="90T1" sheetId="4" r:id="rId7"/>
+    <sheet name="150T1" sheetId="5" r:id="rId8"/>
     <sheet name="30Trial2" sheetId="7" r:id="rId9"/>
     <sheet name="50Trial2" sheetId="8" r:id="rId10"/>
     <sheet name="70Trial2" sheetId="9" r:id="rId11"/>
@@ -4374,7 +4374,7 @@
         <v>30</v>
       </c>
       <c r="B2">
-        <f>'30'!F2</f>
+        <f>'30T1'!F2</f>
         <v>30.016686938266041</v>
       </c>
     </row>
@@ -4383,7 +4383,7 @@
         <v>50</v>
       </c>
       <c r="B3">
-        <f>'50'!F2</f>
+        <f>'50T1'!F2</f>
         <v>50.016859206208871</v>
       </c>
     </row>
@@ -4392,7 +4392,7 @@
         <v>70</v>
       </c>
       <c r="B4">
-        <f>'70'!F2</f>
+        <f>'70T1'!F2</f>
         <v>69.979420256337349</v>
       </c>
     </row>
@@ -4401,7 +4401,7 @@
         <v>90</v>
       </c>
       <c r="B5">
-        <f>'90'!F2</f>
+        <f>'90T1'!F2</f>
         <v>89.936631472127829</v>
       </c>
     </row>
@@ -4410,7 +4410,7 @@
         <v>150</v>
       </c>
       <c r="B6">
-        <f>'150'!F2</f>
+        <f>'150T1'!F2</f>
         <v>149.98617017628763</v>
       </c>
     </row>
@@ -14640,7 +14640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -17813,8 +17813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Just a glance over before tomorrow's meeting
</commit_message>
<xml_diff>
--- a/RPM_verification/RPM_data.xlsx
+++ b/RPM_verification/RPM_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -789,6 +789,21 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:strRef>
               <c:f>Summary!$A:$A</c:f>
@@ -1310,6 +1325,21 @@
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -4352,7 +4382,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6502,7 +6532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -17813,8 +17843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -18702,7 +18732,7 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>